<commit_message>
Updated to PHREEQC3 12386
git-svn-id: svn://136.177.114.72/svn_GW/phreeqc3/branches/concrete@12387 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/Clara-PEST/00_kin_20160528.xlsx
+++ b/Clara-PEST/00_kin_20160528.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fails" sheetId="10" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="80">
   <si>
     <t>pchl</t>
   </si>
@@ -205,9 +205,6 @@
     <t>line in other_outputs.txt</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>relative</t>
   </si>
   <si>
@@ -221,6 +218,51 @@
   </si>
   <si>
     <t>converted to model units</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>pclinop-sr</t>
+  </si>
+  <si>
+    <t>pclinop</t>
+  </si>
+  <si>
+    <t>achl</t>
+  </si>
+  <si>
+    <t>aalb</t>
+  </si>
+  <si>
+    <t>aan</t>
+  </si>
+  <si>
+    <t>aclinop-na</t>
+  </si>
+  <si>
+    <t>aclinop-k</t>
+  </si>
+  <si>
+    <t>aclinop-sr</t>
+  </si>
+  <si>
+    <t>aclinop</t>
+  </si>
+  <si>
+    <t>aash</t>
+  </si>
+  <si>
+    <t>aoliv</t>
+  </si>
+  <si>
+    <t>apyrox</t>
+  </si>
+  <si>
+    <t>aqz</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
@@ -565,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -979,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L26"/>
+  <dimension ref="A2:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,7 +1044,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1351,10 +1393,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" t="s">
         <v>64</v>
-      </c>
-      <c r="L18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1362,13 +1404,13 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
       <c r="D19">
-        <v>4.34</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1377,7 +1419,7 @@
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H19" s="1">
         <v>0.66669999999999996</v>
@@ -1390,57 +1432,38 @@
       </c>
       <c r="L19" s="1">
         <f>D19*H19+I19</f>
-        <v>-7.7765219999999999</v>
+        <v>-10.003299999999999</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
       <c r="D20">
-        <v>9.18</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>10</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="I20" s="1">
-        <v>-7.3330000000000002</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" ref="L20:L26" si="0">D20*H20+I20</f>
-        <v>-4.2733059999999998</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
       <c r="D21">
-        <v>9.75</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1449,34 +1472,34 @@
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" s="1">
-        <v>0.4</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="I21" s="1">
-        <v>-7.4</v>
+        <v>-7.3330000000000002</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="0"/>
-        <v>-3.5</v>
+        <f t="shared" ref="L21:L29" si="0">D21*H21+I21</f>
+        <v>-6.9996999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
       <c r="D22">
-        <v>4.87</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1485,106 +1508,68 @@
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H22" s="1">
-        <v>0.66669999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="I22" s="1">
-        <v>-10.67</v>
+        <v>-7.4</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="0"/>
-        <v>-7.423171</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
       <c r="D23">
-        <v>4.18</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>10</v>
-      </c>
-      <c r="G23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.66669999999999996</v>
-      </c>
-      <c r="I23" s="1">
-        <v>-10.67</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="L23" s="1">
-        <f t="shared" si="0"/>
-        <v>-7.8831940000000005</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
         <v>60</v>
       </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
       <c r="D24">
-        <v>5.43</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>10</v>
-      </c>
-      <c r="G24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0.44440000000000002</v>
-      </c>
-      <c r="I24" s="1">
-        <v>-8.4440000000000008</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="L24" s="1">
-        <f t="shared" si="0"/>
-        <v>-6.030908000000001</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
-        <v>61</v>
-      </c>
       <c r="D25">
-        <v>6.85</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1593,34 +1578,34 @@
         <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1">
-        <v>0.44440000000000002</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="I25" s="1">
-        <v>-8.4440000000000008</v>
+        <v>-10.67</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="0"/>
-        <v>-5.3998600000000003</v>
+        <v>-10.003299999999999</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
         <v>60</v>
       </c>
-      <c r="C26" t="s">
-        <v>61</v>
-      </c>
       <c r="D26">
-        <v>8.2899999999999991</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1629,20 +1614,211 @@
         <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="I26" s="1">
+        <v>-10.67</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="0"/>
+        <v>-10.003299999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1">
         <v>0.44440000000000002</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I27" s="1">
         <v>-8.4440000000000008</v>
       </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1">
-        <f t="shared" si="0"/>
-        <v>-4.7599240000000016</v>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.9996000000000009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="I28" s="1">
+        <v>-8.4440000000000008</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.9996000000000009</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-8.4440000000000008</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.9996000000000009</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37">
+        <v>21.5</v>
+      </c>
+      <c r="H37">
+        <v>1.37</v>
+      </c>
+      <c r="I37">
+        <f>H37*G37</f>
+        <v>29.455000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I38">
+        <f>H38*G38</f>
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39">
+        <f>I38+I37</f>
+        <v>50.155000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40">
+        <f>I39/(G37+G38)</f>
+        <v>1.8926415094339624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>